<commit_message>
Updated telem with read_write flag access
</commit_message>
<xml_diff>
--- a/docs/dRehm_typedefs.xlsx
+++ b/docs/dRehm_typedefs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f79c5810e0243ad1/Arduino/SilF4ware_test/OAVware_uvos_08/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\UAVware\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="292" documentId="8_{FB8021EE-D321-4D2D-BCE4-34A9D857C7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE242C9A-4DFF-4266-B66A-E93E87F76C2B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95913B03-BE88-4C93-BCD6-C2C7B473AFFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AB9256D6-FFE7-42EA-8970-173E847FD94F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{AB9256D6-FFE7-42EA-8970-173E847FD94F}"/>
   </bookViews>
   <sheets>
     <sheet name="CONFIG_STRUCT" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="134">
   <si>
     <t>uint8_t</t>
   </si>
@@ -428,6 +428,15 @@
   </si>
   <si>
     <t>z_Save</t>
+  </si>
+  <si>
+    <t>.read_write =</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
@@ -486,17 +495,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -840,7 +839,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
@@ -1819,12 +1818,12 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F53 F55:F1048576">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="  //">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="  //">
       <formula>NOT(ISERROR(SEARCH("  //",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1840,11 +1839,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95D306D-0130-49BE-A503-AF0145E44D12}">
-  <dimension ref="A1:O54"/>
+  <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="K54" sqref="K54"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1860,9 +1857,12 @@
     <col min="12" max="12" width="2.77734375" customWidth="1"/>
     <col min="13" max="13" width="12.44140625" customWidth="1"/>
     <col min="14" max="14" width="24.6640625" customWidth="1"/>
+    <col min="15" max="15" width="2.77734375" customWidth="1"/>
+    <col min="16" max="16" width="12.44140625" customWidth="1"/>
+    <col min="17" max="17" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="F1" t="s">
         <v>125</v>
       </c>
@@ -1872,11 +1872,14 @@
       <c r="M1" t="s">
         <v>126</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
+        <v>131</v>
+      </c>
+      <c r="R1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>122</v>
       </c>
@@ -1928,12 +1931,23 @@
       <c r="N4" t="s">
         <v>24</v>
       </c>
-      <c r="O4" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E4),O$1,"")</f>
+      <c r="O4" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E4),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P4" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E4),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="R4" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E4),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="F5" t="str">
         <f>IF(ISTEXT(CONFIG_STRUCT!E5),$F$1&amp;CONFIG_STRUCT!E5,"")</f>
         <v/>
@@ -1966,12 +1980,20 @@
         <f>IF(ISTEXT(CONFIG_STRUCT!E5),M$1,"")</f>
         <v/>
       </c>
-      <c r="O5" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E5),O$1,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O5" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E5),",","")</f>
+        <v/>
+      </c>
+      <c r="P5" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E5),P$1,"")</f>
+        <v/>
+      </c>
+      <c r="R5" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E5),R$1,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="F6" t="str">
         <f>IF(ISTEXT(CONFIG_STRUCT!#REF!),$F$1&amp;CONFIG_STRUCT!#REF!,"")</f>
         <v/>
@@ -2004,12 +2026,20 @@
         <f>IF(ISTEXT(CONFIG_STRUCT!E6),M$1,"")</f>
         <v/>
       </c>
-      <c r="O6" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E6),O$1,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O6" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E6),",","")</f>
+        <v/>
+      </c>
+      <c r="P6" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E6),P$1,"")</f>
+        <v/>
+      </c>
+      <c r="R6" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E6),R$1,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>122</v>
       </c>
@@ -2061,12 +2091,23 @@
       <c r="N7" t="s">
         <v>28</v>
       </c>
-      <c r="O7" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E7),O$1,"")</f>
+      <c r="O7" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E7),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P7" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E7),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R7" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E7),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>122</v>
       </c>
@@ -2118,12 +2159,23 @@
       <c r="N8" t="s">
         <v>28</v>
       </c>
-      <c r="O8" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E8),O$1,"")</f>
+      <c r="O8" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E8),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P8" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E8),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R8" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E8),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>122</v>
       </c>
@@ -2175,12 +2227,23 @@
       <c r="N9" t="s">
         <v>28</v>
       </c>
-      <c r="O9" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E9),O$1,"")</f>
+      <c r="O9" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E9),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P9" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E9),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R9" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E9),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -2232,12 +2295,23 @@
       <c r="N10" t="s">
         <v>28</v>
       </c>
-      <c r="O10" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E10),O$1,"")</f>
+      <c r="O10" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E10),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P10" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E10),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R10" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E10),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>122</v>
       </c>
@@ -2289,12 +2363,23 @@
       <c r="N11" t="s">
         <v>28</v>
       </c>
-      <c r="O11" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E11),O$1,"")</f>
+      <c r="O11" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E11),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P11" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E11),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R11" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E11),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>122</v>
       </c>
@@ -2346,12 +2431,23 @@
       <c r="N12" t="s">
         <v>28</v>
       </c>
-      <c r="O12" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E12),O$1,"")</f>
+      <c r="O12" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E12),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P12" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E12),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R12" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E12),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D13" s="3"/>
       <c r="G13" s="3" t="str">
         <f>IF(ISTEXT(CONFIG_STRUCT!D13),"=","")</f>
@@ -2381,12 +2477,21 @@
         <f>IF(ISTEXT(CONFIG_STRUCT!E13),M$1,"")</f>
         <v/>
       </c>
-      <c r="O13" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E13),O$1,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O13" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E13),",","")</f>
+        <v/>
+      </c>
+      <c r="P13" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E13),P$1,"")</f>
+        <v/>
+      </c>
+      <c r="Q13" s="3"/>
+      <c r="R13" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E13),R$1,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D14" s="3"/>
       <c r="G14" s="3" t="str">
         <f>IF(ISTEXT(CONFIG_STRUCT!D14),"=","")</f>
@@ -2416,12 +2521,21 @@
         <f>IF(ISTEXT(CONFIG_STRUCT!E14),M$1,"")</f>
         <v/>
       </c>
-      <c r="O14" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E14),O$1,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O14" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E14),",","")</f>
+        <v/>
+      </c>
+      <c r="P14" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E14),P$1,"")</f>
+        <v/>
+      </c>
+      <c r="Q14" s="3"/>
+      <c r="R14" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E14),R$1,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>122</v>
       </c>
@@ -2473,17 +2587,28 @@
       <c r="N15" t="s">
         <v>32</v>
       </c>
-      <c r="O15" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E15),O$1,"")</f>
+      <c r="O15" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E15),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P15" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E15),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q15" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R15" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E15),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>122</v>
       </c>
       <c r="B16">
-        <f t="shared" ref="B16:B54" si="1">B15+1</f>
+        <f t="shared" ref="B16:B52" si="1">B15+1</f>
         <v>8</v>
       </c>
       <c r="C16" t="s">
@@ -2530,12 +2655,23 @@
       <c r="N16" t="s">
         <v>32</v>
       </c>
-      <c r="O16" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E16),O$1,"")</f>
+      <c r="O16" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E16),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P16" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E16),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R16" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E16),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>122</v>
       </c>
@@ -2587,12 +2723,23 @@
       <c r="N17" t="s">
         <v>32</v>
       </c>
-      <c r="O17" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E17),O$1,"")</f>
+      <c r="O17" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E17),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P17" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E17),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q17" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R17" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E17),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>122</v>
       </c>
@@ -2644,12 +2791,23 @@
       <c r="N18" t="s">
         <v>32</v>
       </c>
-      <c r="O18" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E18),O$1,"")</f>
+      <c r="O18" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E18),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P18" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E18),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q18" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R18" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E18),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D19" s="3"/>
       <c r="G19" s="3" t="str">
         <f>IF(ISTEXT(CONFIG_STRUCT!D19),"=","")</f>
@@ -2679,12 +2837,21 @@
         <f>IF(ISTEXT(CONFIG_STRUCT!E19),M$1,"")</f>
         <v/>
       </c>
-      <c r="O19" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E19),O$1,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O19" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E19),",","")</f>
+        <v/>
+      </c>
+      <c r="P19" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E19),P$1,"")</f>
+        <v/>
+      </c>
+      <c r="Q19" s="3"/>
+      <c r="R19" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E19),R$1,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D20" s="3"/>
       <c r="G20" s="3" t="str">
         <f>IF(ISTEXT(CONFIG_STRUCT!D20),"=","")</f>
@@ -2714,12 +2881,21 @@
         <f>IF(ISTEXT(CONFIG_STRUCT!E20),M$1,"")</f>
         <v/>
       </c>
-      <c r="O20" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E20),O$1,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O20" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E20),",","")</f>
+        <v/>
+      </c>
+      <c r="P20" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E20),P$1,"")</f>
+        <v/>
+      </c>
+      <c r="Q20" s="3"/>
+      <c r="R20" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E20),R$1,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>122</v>
       </c>
@@ -2771,12 +2947,23 @@
       <c r="N21" t="s">
         <v>32</v>
       </c>
-      <c r="O21" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E21),O$1,"")</f>
+      <c r="O21" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E21),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P21" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E21),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q21" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R21" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E21),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>122</v>
       </c>
@@ -2828,12 +3015,23 @@
       <c r="N22" t="s">
         <v>32</v>
       </c>
-      <c r="O22" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E22),O$1,"")</f>
+      <c r="O22" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E22),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P22" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E22),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q22" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R22" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E22),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>122</v>
       </c>
@@ -2885,12 +3083,23 @@
       <c r="N23" t="s">
         <v>32</v>
       </c>
-      <c r="O23" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E23),O$1,"")</f>
+      <c r="O23" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E23),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P23" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E23),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q23" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R23" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E23),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>122</v>
       </c>
@@ -2942,12 +3151,23 @@
       <c r="N24" t="s">
         <v>32</v>
       </c>
-      <c r="O24" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E24),O$1,"")</f>
+      <c r="O24" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E24),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P24" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E24),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q24" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R24" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E24),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>122</v>
       </c>
@@ -2999,12 +3219,23 @@
       <c r="N25" t="s">
         <v>32</v>
       </c>
-      <c r="O25" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E25),O$1,"")</f>
+      <c r="O25" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E25),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P25" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E25),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q25" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R25" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E25),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>122</v>
       </c>
@@ -3056,12 +3287,23 @@
       <c r="N26" t="s">
         <v>32</v>
       </c>
-      <c r="O26" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E26),O$1,"")</f>
+      <c r="O26" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E26),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P26" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E26),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q26" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R26" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E26),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D27" s="3"/>
       <c r="G27" s="3" t="str">
         <f>IF(ISTEXT(CONFIG_STRUCT!D27),"=","")</f>
@@ -3091,12 +3333,21 @@
         <f>IF(ISTEXT(CONFIG_STRUCT!E27),M$1,"")</f>
         <v/>
       </c>
-      <c r="O27" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E27),O$1,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O27" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E27),",","")</f>
+        <v/>
+      </c>
+      <c r="P27" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E27),P$1,"")</f>
+        <v/>
+      </c>
+      <c r="Q27" s="3"/>
+      <c r="R27" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E27),R$1,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D28" s="3"/>
       <c r="G28" s="3" t="str">
         <f>IF(ISTEXT(CONFIG_STRUCT!D28),"=","")</f>
@@ -3126,12 +3377,21 @@
         <f>IF(ISTEXT(CONFIG_STRUCT!E28),M$1,"")</f>
         <v/>
       </c>
-      <c r="O28" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E28),O$1,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O28" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E28),",","")</f>
+        <v/>
+      </c>
+      <c r="P28" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E28),P$1,"")</f>
+        <v/>
+      </c>
+      <c r="Q28" s="3"/>
+      <c r="R28" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E28),R$1,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>122</v>
       </c>
@@ -3183,12 +3443,23 @@
       <c r="N29" t="s">
         <v>32</v>
       </c>
-      <c r="O29" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E29),O$1,"")</f>
+      <c r="O29" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E29),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P29" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E29),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q29" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R29" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E29),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>122</v>
       </c>
@@ -3240,12 +3511,23 @@
       <c r="N30" t="s">
         <v>32</v>
       </c>
-      <c r="O30" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E30),O$1,"")</f>
+      <c r="O30" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E30),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P30" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E30),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q30" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R30" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E30),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>122</v>
       </c>
@@ -3297,12 +3579,23 @@
       <c r="N31" t="s">
         <v>32</v>
       </c>
-      <c r="O31" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E31),O$1,"")</f>
+      <c r="O31" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E31),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P31" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E31),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q31" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R31" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E31),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>122</v>
       </c>
@@ -3354,12 +3647,23 @@
       <c r="N32" t="s">
         <v>32</v>
       </c>
-      <c r="O32" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E32),O$1,"")</f>
+      <c r="O32" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E32),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P32" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E32),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q32" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R32" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E32),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D33" s="3"/>
       <c r="G33" s="3" t="str">
         <f>IF(ISTEXT(CONFIG_STRUCT!D33),"=","")</f>
@@ -3389,12 +3693,21 @@
         <f>IF(ISTEXT(CONFIG_STRUCT!E33),M$1,"")</f>
         <v/>
       </c>
-      <c r="O33" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E33),O$1,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O33" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E33),",","")</f>
+        <v/>
+      </c>
+      <c r="P33" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E33),P$1,"")</f>
+        <v/>
+      </c>
+      <c r="Q33" s="3"/>
+      <c r="R33" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E33),R$1,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>122</v>
       </c>
@@ -3446,12 +3759,23 @@
       <c r="N34" t="s">
         <v>32</v>
       </c>
-      <c r="O34" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E34),O$1,"")</f>
+      <c r="O34" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E34),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P34" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E34),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q34" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R34" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E34),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>122</v>
       </c>
@@ -3503,12 +3827,23 @@
       <c r="N35" t="s">
         <v>32</v>
       </c>
-      <c r="O35" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E35),O$1,"")</f>
+      <c r="O35" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E35),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P35" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E35),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q35" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R35" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E35),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>122</v>
       </c>
@@ -3560,12 +3895,23 @@
       <c r="N36" t="s">
         <v>32</v>
       </c>
-      <c r="O36" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E36),O$1,"")</f>
+      <c r="O36" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E36),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P36" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E36),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q36" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R36" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E36),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>122</v>
       </c>
@@ -3617,12 +3963,23 @@
       <c r="N37" t="s">
         <v>32</v>
       </c>
-      <c r="O37" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E37),O$1,"")</f>
+      <c r="O37" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E37),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P37" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E37),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q37" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R37" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E37),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>122</v>
       </c>
@@ -3674,12 +4031,23 @@
       <c r="N38" t="s">
         <v>32</v>
       </c>
-      <c r="O38" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E38),O$1,"")</f>
+      <c r="O38" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E38),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P38" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E38),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q38" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R38" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E38),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>122</v>
       </c>
@@ -3731,12 +4099,23 @@
       <c r="N39" t="s">
         <v>32</v>
       </c>
-      <c r="O39" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E39),O$1,"")</f>
+      <c r="O39" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E39),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P39" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E39),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q39" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R39" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E39),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>122</v>
       </c>
@@ -3788,12 +4167,23 @@
       <c r="N40" t="s">
         <v>32</v>
       </c>
-      <c r="O40" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E40),O$1,"")</f>
+      <c r="O40" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E40),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P40" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E40),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q40" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R40" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E40),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>122</v>
       </c>
@@ -3845,12 +4235,23 @@
       <c r="N41" t="s">
         <v>32</v>
       </c>
-      <c r="O41" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E41),O$1,"")</f>
+      <c r="O41" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E41),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P41" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E41),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q41" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R41" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E41),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D42" s="3"/>
       <c r="G42" s="3" t="str">
         <f>IF(ISTEXT(CONFIG_STRUCT!D42),"=","")</f>
@@ -3880,12 +4281,21 @@
         <f>IF(ISTEXT(CONFIG_STRUCT!E42),M$1,"")</f>
         <v/>
       </c>
-      <c r="O42" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E42),O$1,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O42" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E42),",","")</f>
+        <v/>
+      </c>
+      <c r="P42" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E42),P$1,"")</f>
+        <v/>
+      </c>
+      <c r="Q42" s="3"/>
+      <c r="R42" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E42),R$1,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>122</v>
       </c>
@@ -3937,12 +4347,23 @@
       <c r="N43" t="s">
         <v>32</v>
       </c>
-      <c r="O43" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E43),O$1,"")</f>
+      <c r="O43" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E43),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P43" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E43),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q43" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R43" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E43),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>122</v>
       </c>
@@ -3994,12 +4415,23 @@
       <c r="N44" t="s">
         <v>32</v>
       </c>
-      <c r="O44" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E44),O$1,"")</f>
+      <c r="O44" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E44),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P44" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E44),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q44" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R44" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E44),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>122</v>
       </c>
@@ -4051,12 +4483,23 @@
       <c r="N45" t="s">
         <v>32</v>
       </c>
-      <c r="O45" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E45),O$1,"")</f>
+      <c r="O45" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E45),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P45" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E45),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q45" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R45" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E45),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>122</v>
       </c>
@@ -4108,12 +4551,23 @@
       <c r="N46" t="s">
         <v>32</v>
       </c>
-      <c r="O46" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E46),O$1,"")</f>
+      <c r="O46" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E46),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P46" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E46),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q46" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R46" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E46),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>122</v>
       </c>
@@ -4165,12 +4619,23 @@
       <c r="N47" t="s">
         <v>32</v>
       </c>
-      <c r="O47" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E47),O$1,"")</f>
+      <c r="O47" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E47),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P47" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E47),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q47" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R47" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E47),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>122</v>
       </c>
@@ -4222,12 +4687,23 @@
       <c r="N48" t="s">
         <v>32</v>
       </c>
-      <c r="O48" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E48),O$1,"")</f>
+      <c r="O48" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E48),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P48" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E48),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q48" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R48" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E48),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D49" s="3"/>
       <c r="G49" s="3" t="str">
         <f>IF(ISTEXT(CONFIG_STRUCT!D49),"=","")</f>
@@ -4257,12 +4733,21 @@
         <f>IF(ISTEXT(CONFIG_STRUCT!E49),M$1,"")</f>
         <v/>
       </c>
-      <c r="O49" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E49),O$1,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O49" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E49),",","")</f>
+        <v/>
+      </c>
+      <c r="P49" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E49),P$1,"")</f>
+        <v/>
+      </c>
+      <c r="Q49" s="3"/>
+      <c r="R49" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E49),R$1,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>122</v>
       </c>
@@ -4314,12 +4799,23 @@
       <c r="N50" t="s">
         <v>32</v>
       </c>
-      <c r="O50" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E50),O$1,"")</f>
+      <c r="O50" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E50),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P50" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E50),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q50" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R50" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E50),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>122</v>
       </c>
@@ -4371,12 +4867,23 @@
       <c r="N51" t="s">
         <v>32</v>
       </c>
-      <c r="O51" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E51),O$1,"")</f>
+      <c r="O51" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E51),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P51" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E51),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q51" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R51" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E51),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>122</v>
       </c>
@@ -4428,18 +4935,38 @@
       <c r="N52" t="s">
         <v>32</v>
       </c>
-      <c r="O52" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E52),O$1,"")</f>
+      <c r="O52" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E52),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P52" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E52),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q52" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R52" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E52),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D53" s="3"/>
       <c r="G53" s="3"/>
       <c r="I53" s="3"/>
       <c r="L53" s="3"/>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O53" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E53),",","")</f>
+        <v/>
+      </c>
+      <c r="P53" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E53),P$1,"")</f>
+        <v/>
+      </c>
+      <c r="Q53" s="3"/>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>122</v>
       </c>
@@ -4491,8 +5018,19 @@
       <c r="N54" t="s">
         <v>24</v>
       </c>
-      <c r="O54" t="str">
-        <f>IF(ISTEXT(CONFIG_STRUCT!E54),O$1,"")</f>
+      <c r="O54" s="3" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E54),",","")</f>
+        <v>,</v>
+      </c>
+      <c r="P54" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E54),P$1,"")</f>
+        <v>.read_write =</v>
+      </c>
+      <c r="Q54" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R54" t="str">
+        <f>IF(ISTEXT(CONFIG_STRUCT!E54),R$1,"")</f>
         <v xml:space="preserve">  },</v>
       </c>
     </row>

</xml_diff>